<commit_message>
Added new css files for datepicker and sb-admin layout
</commit_message>
<xml_diff>
--- a/templates/penelitian_dosen_template.xlsx
+++ b/templates/penelitian_dosen_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericanthony/Projects/nodejs-fullstack/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26482E1-803C-9C41-B5ED-E1F6F29500FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3389F4-5FC6-1644-A725-97BAF2A0A2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17580" xr2:uid="{8BB63F20-05C5-C047-9481-25E0B1F899C8}"/>
+    <workbookView xWindow="4880" yWindow="760" windowWidth="25800" windowHeight="17580" xr2:uid="{8BB63F20-05C5-C047-9481-25E0B1F899C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>judul_proposal</t>
-  </si>
-  <si>
     <t>biaya_yang_diajukan</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>825200050,825200049</t>
+  </si>
+  <si>
+    <t>judul</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,36 +485,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4">
         <v>133860000</v>
@@ -529,16 +529,16 @@
         <v>2021</v>
       </c>
       <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>